<commit_message>
Updated Sphinx documentation and updated Gantt Chart
</commit_message>
<xml_diff>
--- a/Gantt Charts/Milestone2-GanttChart.xlsx
+++ b/Gantt Charts/Milestone2-GanttChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shana/Desktop/CMPE 131/calApp/Calendar-Scheduling-App-master/Gantt Charts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/de594e4e93e79e7e/Documents/Spring2020/CMPE 131/project/Calendar-Scheduling-app/Gantt Charts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015F4838-0B26-E54F-9413-8DDD1BD8084A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{015F4838-0B26-E54F-9413-8DDD1BD8084A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F72D0CBE-E9BB-4966-B2EA-4E931021CABE}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="620" windowWidth="26240" windowHeight="16900" xr2:uid="{AA7B69DF-3B17-C04C-9150-938323FE9379}"/>
+    <workbookView xWindow="2123" yWindow="2242" windowWidth="16874" windowHeight="10523" xr2:uid="{AA7B69DF-3B17-C04C-9150-938323FE9379}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -634,9 +634,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="13" applyFont="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -646,12 +643,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="15" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -720,21 +711,6 @@
     </xf>
     <xf numFmtId="16" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -802,6 +778,30 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -1135,142 +1135,142 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382B5C2B-D08E-CD4E-BF62-F343AB5B8050}">
   <dimension ref="A1:BN173"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" style="4" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="4" customWidth="1"/>
-    <col min="4" max="6" width="10.83203125" style="4"/>
-    <col min="7" max="7" width="7.6640625" style="4" customWidth="1"/>
-    <col min="8" max="66" width="8.83203125" style="4" customWidth="1"/>
-    <col min="67" max="68" width="5.33203125" style="4" customWidth="1"/>
-    <col min="69" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="17.1875" style="4" customWidth="1"/>
+    <col min="2" max="3" width="10.8125" style="4" customWidth="1"/>
+    <col min="4" max="6" width="10.8125" style="4"/>
+    <col min="7" max="7" width="7.6875" style="4" customWidth="1"/>
+    <col min="8" max="66" width="8.8125" style="4" customWidth="1"/>
+    <col min="67" max="68" width="5.3125" style="4" customWidth="1"/>
+    <col min="69" max="16384" width="10.8125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="34" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:66" s="54" customFormat="1" ht="64.05" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="35"/>
-      <c r="AF1" s="35"/>
-      <c r="AG1" s="35"/>
-      <c r="AH1" s="35"/>
-      <c r="AI1" s="35"/>
-      <c r="AJ1" s="35"/>
-      <c r="AK1" s="35"/>
-      <c r="AL1" s="35"/>
-      <c r="AM1" s="35"/>
-      <c r="AN1" s="35"/>
-      <c r="AO1" s="35"/>
-      <c r="AP1" s="35"/>
-      <c r="AQ1" s="35"/>
-      <c r="AR1" s="35"/>
-      <c r="AS1" s="35"/>
-      <c r="AT1" s="35"/>
-      <c r="AU1" s="35"/>
-      <c r="AV1" s="35"/>
-      <c r="AW1" s="35"/>
-      <c r="AX1" s="35"/>
-      <c r="AY1" s="35"/>
-      <c r="AZ1" s="35"/>
-      <c r="BA1" s="35"/>
-      <c r="BB1" s="35"/>
-      <c r="BC1" s="35"/>
-      <c r="BD1" s="35"/>
-      <c r="BE1" s="35"/>
-      <c r="BF1" s="35"/>
-      <c r="BG1" s="35"/>
-      <c r="BH1" s="35"/>
-      <c r="BI1" s="35"/>
-      <c r="BJ1" s="35"/>
-      <c r="BK1" s="35"/>
-      <c r="BL1" s="35"/>
-      <c r="BM1" s="35"/>
-      <c r="BN1" s="35"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
+      <c r="X1" s="55"/>
+      <c r="Y1" s="55"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="55"/>
+      <c r="AC1" s="55"/>
+      <c r="AD1" s="55"/>
+      <c r="AE1" s="55"/>
+      <c r="AF1" s="55"/>
+      <c r="AG1" s="55"/>
+      <c r="AH1" s="55"/>
+      <c r="AI1" s="55"/>
+      <c r="AJ1" s="55"/>
+      <c r="AK1" s="55"/>
+      <c r="AL1" s="55"/>
+      <c r="AM1" s="55"/>
+      <c r="AN1" s="55"/>
+      <c r="AO1" s="55"/>
+      <c r="AP1" s="55"/>
+      <c r="AQ1" s="55"/>
+      <c r="AR1" s="55"/>
+      <c r="AS1" s="55"/>
+      <c r="AT1" s="55"/>
+      <c r="AU1" s="55"/>
+      <c r="AV1" s="55"/>
+      <c r="AW1" s="55"/>
+      <c r="AX1" s="55"/>
+      <c r="AY1" s="55"/>
+      <c r="AZ1" s="55"/>
+      <c r="BA1" s="55"/>
+      <c r="BB1" s="55"/>
+      <c r="BC1" s="55"/>
+      <c r="BD1" s="55"/>
+      <c r="BE1" s="55"/>
+      <c r="BF1" s="55"/>
+      <c r="BG1" s="55"/>
+      <c r="BH1" s="55"/>
+      <c r="BI1" s="55"/>
+      <c r="BJ1" s="55"/>
+      <c r="BK1" s="55"/>
+      <c r="BL1" s="55"/>
+      <c r="BM1" s="55"/>
+      <c r="BN1" s="55"/>
     </row>
-    <row r="2" spans="1:66" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+    <row r="2" spans="1:66" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="17" t="s">
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="18" t="s">
+      <c r="I2" s="17"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="19"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="17" t="s">
+      <c r="L2" s="16"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="20"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="30" t="s">
+      <c r="O2" s="17"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="21"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="25" t="s">
+      <c r="R2" s="18"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22"/>
-      <c r="AE2" s="22"/>
-      <c r="AF2" s="23"/>
-      <c r="AG2" s="22"/>
-      <c r="AH2" s="21"/>
-      <c r="AI2" s="22"/>
-      <c r="AJ2" s="22"/>
-      <c r="AK2" s="22"/>
-      <c r="AL2" s="22"/>
-      <c r="AM2" s="22"/>
-      <c r="AN2" s="22"/>
-      <c r="AO2" s="22"/>
+      <c r="Y2" s="29"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="19"/>
+      <c r="AH2" s="18"/>
+      <c r="AI2" s="19"/>
+      <c r="AJ2" s="19"/>
+      <c r="AK2" s="19"/>
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="19"/>
+      <c r="AO2" s="19"/>
       <c r="AP2" s="3"/>
       <c r="AQ2" s="3"/>
       <c r="AR2" s="3"/>
@@ -1297,183 +1297,183 @@
       <c r="BM2" s="3"/>
       <c r="BN2" s="3"/>
     </row>
-    <row r="3" spans="1:66" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:66" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-      <c r="AC3" s="8"/>
-      <c r="AD3" s="8"/>
-      <c r="AE3" s="8"/>
-      <c r="AF3" s="8"/>
-      <c r="AG3" s="8"/>
-      <c r="AH3" s="8"/>
-      <c r="AI3" s="8"/>
-      <c r="AJ3" s="8"/>
-      <c r="AK3" s="8"/>
-      <c r="AL3" s="8"/>
-      <c r="AM3" s="8"/>
-      <c r="AN3" s="8"/>
-      <c r="AO3" s="8"/>
-      <c r="AP3" s="8"/>
-      <c r="AQ3" s="8"/>
-      <c r="AR3" s="8"/>
-      <c r="AS3" s="8"/>
-      <c r="AT3" s="8"/>
-      <c r="AU3" s="8"/>
-      <c r="AV3" s="8"/>
-      <c r="AW3" s="8"/>
-      <c r="AX3" s="8"/>
-      <c r="AY3" s="8"/>
-      <c r="AZ3" s="8"/>
-      <c r="BA3" s="8"/>
-      <c r="BB3" s="8"/>
-      <c r="BC3" s="8"/>
-      <c r="BD3" s="8"/>
-      <c r="BE3" s="8"/>
-      <c r="BF3" s="8"/>
-      <c r="BG3" s="8"/>
-      <c r="BH3" s="8"/>
-      <c r="BI3" s="8"/>
-      <c r="BJ3" s="8"/>
-      <c r="BK3" s="8"/>
-      <c r="BL3" s="8"/>
-      <c r="BM3" s="8"/>
-      <c r="BN3" s="8"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="7"/>
+      <c r="AI3" s="7"/>
+      <c r="AJ3" s="7"/>
+      <c r="AK3" s="7"/>
+      <c r="AL3" s="7"/>
+      <c r="AM3" s="7"/>
+      <c r="AN3" s="7"/>
+      <c r="AO3" s="7"/>
+      <c r="AP3" s="7"/>
+      <c r="AQ3" s="7"/>
+      <c r="AR3" s="7"/>
+      <c r="AS3" s="7"/>
+      <c r="AT3" s="7"/>
+      <c r="AU3" s="7"/>
+      <c r="AV3" s="7"/>
+      <c r="AW3" s="7"/>
+      <c r="AX3" s="7"/>
+      <c r="AY3" s="7"/>
+      <c r="AZ3" s="7"/>
+      <c r="BA3" s="7"/>
+      <c r="BB3" s="7"/>
+      <c r="BC3" s="7"/>
+      <c r="BD3" s="7"/>
+      <c r="BE3" s="7"/>
+      <c r="BF3" s="7"/>
+      <c r="BG3" s="7"/>
+      <c r="BH3" s="7"/>
+      <c r="BI3" s="7"/>
+      <c r="BJ3" s="7"/>
+      <c r="BK3" s="7"/>
+      <c r="BL3" s="7"/>
+      <c r="BM3" s="7"/>
+      <c r="BN3" s="7"/>
     </row>
-    <row r="4" spans="1:66" ht="26" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="16">
+    <row r="4" spans="1:66" ht="26" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="61"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="13">
         <v>43934</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="11">
         <v>14</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="11">
         <v>15</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="12">
         <v>16</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="12">
         <v>17</v>
       </c>
-      <c r="L4" s="15">
+      <c r="L4" s="12">
         <v>18</v>
       </c>
-      <c r="M4" s="15">
+      <c r="M4" s="12">
         <v>19</v>
       </c>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="15"/>
-      <c r="AA4" s="15"/>
-      <c r="AB4" s="15"/>
-      <c r="AC4" s="15"/>
-      <c r="AD4" s="15"/>
-      <c r="AE4" s="15"/>
-      <c r="AF4" s="15"/>
-      <c r="AG4" s="15"/>
-      <c r="AH4" s="15"/>
-      <c r="AI4" s="15"/>
-      <c r="AJ4" s="15"/>
-      <c r="AK4" s="15"/>
-      <c r="AL4" s="15"/>
-      <c r="AM4" s="15"/>
-      <c r="AN4" s="15"/>
-      <c r="AO4" s="15"/>
-      <c r="AP4" s="15"/>
-      <c r="AQ4" s="15"/>
-      <c r="AR4" s="15"/>
-      <c r="AS4" s="15"/>
-      <c r="AT4" s="15"/>
-      <c r="AU4" s="15"/>
-      <c r="AV4" s="15"/>
-      <c r="AW4" s="15"/>
-      <c r="AX4" s="15"/>
-      <c r="AY4" s="15"/>
-      <c r="AZ4" s="15"/>
-      <c r="BA4" s="15"/>
-      <c r="BB4" s="15"/>
-      <c r="BC4" s="15"/>
-      <c r="BD4" s="15"/>
-      <c r="BE4" s="15"/>
-      <c r="BF4" s="15"/>
-      <c r="BG4" s="15"/>
-      <c r="BH4" s="15"/>
-      <c r="BI4" s="15"/>
-      <c r="BJ4" s="15"/>
-      <c r="BK4" s="15"/>
-      <c r="BL4" s="15"/>
-      <c r="BM4" s="15"/>
-      <c r="BN4" s="15"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
+      <c r="AA4" s="12"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="12"/>
+      <c r="AD4" s="12"/>
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="12"/>
+      <c r="AG4" s="12"/>
+      <c r="AH4" s="12"/>
+      <c r="AI4" s="12"/>
+      <c r="AJ4" s="12"/>
+      <c r="AK4" s="12"/>
+      <c r="AL4" s="12"/>
+      <c r="AM4" s="12"/>
+      <c r="AN4" s="12"/>
+      <c r="AO4" s="12"/>
+      <c r="AP4" s="12"/>
+      <c r="AQ4" s="12"/>
+      <c r="AR4" s="12"/>
+      <c r="AS4" s="12"/>
+      <c r="AT4" s="12"/>
+      <c r="AU4" s="12"/>
+      <c r="AV4" s="12"/>
+      <c r="AW4" s="12"/>
+      <c r="AX4" s="12"/>
+      <c r="AY4" s="12"/>
+      <c r="AZ4" s="12"/>
+      <c r="BA4" s="12"/>
+      <c r="BB4" s="12"/>
+      <c r="BC4" s="12"/>
+      <c r="BD4" s="12"/>
+      <c r="BE4" s="12"/>
+      <c r="BF4" s="12"/>
+      <c r="BG4" s="12"/>
+      <c r="BH4" s="12"/>
+      <c r="BI4" s="12"/>
+      <c r="BJ4" s="12"/>
+      <c r="BK4" s="12"/>
+      <c r="BL4" s="12"/>
+      <c r="BM4" s="12"/>
+      <c r="BN4" s="12"/>
     </row>
-    <row r="5" spans="1:66" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:66" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="30">
         <v>43935</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="9">
         <v>2</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="9">
         <v>14</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
-      <c r="H5" s="27"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10"/>
+      <c r="H5" s="24"/>
       <c r="I5" s="2"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1533,15 +1533,15 @@
       <c r="BM5" s="3"/>
       <c r="BN5" s="3"/>
     </row>
-    <row r="6" spans="1:66" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="55"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="54"/>
+    <row r="6" spans="1:66" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="47"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="46"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1600,23 +1600,23 @@
       <c r="BM6" s="3"/>
       <c r="BN6" s="3"/>
     </row>
-    <row r="7" spans="1:66" ht="38" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:66" ht="33.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="9">
         <v>15</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="9">
         <v>1</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="9">
         <v>15</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="27"/>
+      <c r="I7" s="24"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1675,19 +1675,19 @@
       <c r="BM7" s="3"/>
       <c r="BN7" s="3"/>
     </row>
-    <row r="8" spans="1:66" ht="38" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:66" ht="33.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="9">
         <v>15</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="9">
         <v>3</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10"/>
       <c r="H8" s="1"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1748,19 +1748,19 @@
       <c r="BM8" s="3"/>
       <c r="BN8" s="3"/>
     </row>
-    <row r="9" spans="1:66" ht="38" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:66" ht="33.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="9">
         <v>15</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="9">
         <v>3</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
       <c r="H9" s="1"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1772,7 +1772,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
-      <c r="S9" s="24"/>
+      <c r="S9" s="21"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
@@ -1821,17 +1821,17 @@
       <c r="BM9" s="3"/>
       <c r="BN9" s="3"/>
     </row>
-    <row r="10" spans="1:66" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
+    <row r="10" spans="1:66" ht="16.899999999999999" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -1839,7 +1839,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
-      <c r="S10" s="53"/>
+      <c r="S10" s="45"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
@@ -1888,25 +1888,25 @@
       <c r="BM10" s="3"/>
       <c r="BN10" s="3"/>
     </row>
-    <row r="11" spans="1:66" ht="55" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:66" ht="49.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="9">
         <v>14</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="9">
         <v>1</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="9">
         <v>14</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -1963,19 +1963,19 @@
       <c r="BM11" s="3"/>
       <c r="BN11" s="3"/>
     </row>
-    <row r="12" spans="1:66" ht="74" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:66" ht="66.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="9">
         <v>15</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="9">
         <v>3</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
       <c r="H12" s="1"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -2036,17 +2036,17 @@
       <c r="BM12" s="3"/>
       <c r="BN12" s="3"/>
     </row>
-    <row r="13" spans="1:66" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
+    <row r="13" spans="1:66" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="10"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="59"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="51"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -2103,25 +2103,25 @@
       <c r="BM13" s="3"/>
       <c r="BN13" s="3"/>
     </row>
-    <row r="14" spans="1:66" ht="38" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:66" ht="33.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="9">
         <v>14</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="9">
         <v>2</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="9">
         <v>14</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="H14" s="27"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="H14" s="24"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="53"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="45"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -2178,22 +2178,22 @@
       <c r="BM14" s="3"/>
       <c r="BN14" s="3"/>
     </row>
-    <row r="15" spans="1:66" ht="38" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:66" ht="33.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="9">
         <v>18</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="9">
         <v>1</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="13"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="J15" s="24"/>
       <c r="K15" s="1"/>
       <c r="L15" s="2"/>
       <c r="M15" s="1"/>
@@ -2251,13 +2251,13 @@
       <c r="BM15" s="3"/>
       <c r="BN15" s="3"/>
     </row>
-    <row r="16" spans="1:66" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
+    <row r="16" spans="1:66" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="10"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -2319,129 +2319,129 @@
       <c r="BM16" s="3"/>
       <c r="BN16" s="3"/>
     </row>
-    <row r="17" spans="1:66" s="41" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="42"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="43"/>
-      <c r="M17" s="43"/>
-      <c r="N17" s="43"/>
-      <c r="O17" s="43"/>
-      <c r="P17" s="43"/>
-      <c r="Q17" s="43"/>
-      <c r="R17" s="43"/>
-      <c r="S17" s="43"/>
-      <c r="T17" s="43"/>
-      <c r="U17" s="43"/>
-      <c r="V17" s="43"/>
-      <c r="W17" s="43"/>
-      <c r="X17" s="43"/>
-      <c r="Y17" s="43"/>
-      <c r="Z17" s="43"/>
-      <c r="AA17" s="45"/>
-      <c r="AB17" s="45"/>
-      <c r="AC17" s="45"/>
-      <c r="AD17" s="45"/>
-      <c r="AE17" s="45"/>
-      <c r="AF17" s="45"/>
-      <c r="AG17" s="45"/>
-      <c r="AH17" s="45"/>
-      <c r="AI17" s="45"/>
-      <c r="AJ17" s="45"/>
-      <c r="AK17" s="45"/>
-      <c r="AL17" s="45"/>
-      <c r="AM17" s="45"/>
-      <c r="AN17" s="45"/>
-      <c r="AO17" s="45"/>
-      <c r="AP17" s="45"/>
-      <c r="AQ17" s="45"/>
-      <c r="AR17" s="45"/>
-      <c r="AS17" s="45"/>
-      <c r="AT17" s="45"/>
-      <c r="AU17" s="45"/>
-      <c r="AV17" s="45"/>
-      <c r="AW17" s="45"/>
-      <c r="AX17" s="45"/>
-      <c r="AY17" s="45"/>
-      <c r="AZ17" s="45"/>
-      <c r="BA17" s="45"/>
-      <c r="BB17" s="45"/>
-      <c r="BC17" s="45"/>
-      <c r="BD17" s="45"/>
-      <c r="BE17" s="45"/>
-      <c r="BF17" s="45"/>
-      <c r="BG17" s="45"/>
-      <c r="BH17" s="45"/>
-      <c r="BI17" s="45"/>
-      <c r="BJ17" s="45"/>
-      <c r="BK17" s="45"/>
-      <c r="BL17" s="45"/>
-      <c r="BM17" s="45"/>
-      <c r="BN17" s="40"/>
+    <row r="17" spans="1:66" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="34"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="35"/>
+      <c r="S17" s="35"/>
+      <c r="T17" s="35"/>
+      <c r="U17" s="35"/>
+      <c r="V17" s="35"/>
+      <c r="W17" s="35"/>
+      <c r="X17" s="35"/>
+      <c r="Y17" s="35"/>
+      <c r="Z17" s="35"/>
+      <c r="AA17" s="37"/>
+      <c r="AB17" s="37"/>
+      <c r="AC17" s="37"/>
+      <c r="AD17" s="37"/>
+      <c r="AE17" s="37"/>
+      <c r="AF17" s="37"/>
+      <c r="AG17" s="37"/>
+      <c r="AH17" s="37"/>
+      <c r="AI17" s="37"/>
+      <c r="AJ17" s="37"/>
+      <c r="AK17" s="37"/>
+      <c r="AL17" s="37"/>
+      <c r="AM17" s="37"/>
+      <c r="AN17" s="37"/>
+      <c r="AO17" s="37"/>
+      <c r="AP17" s="37"/>
+      <c r="AQ17" s="37"/>
+      <c r="AR17" s="37"/>
+      <c r="AS17" s="37"/>
+      <c r="AT17" s="37"/>
+      <c r="AU17" s="37"/>
+      <c r="AV17" s="37"/>
+      <c r="AW17" s="37"/>
+      <c r="AX17" s="37"/>
+      <c r="AY17" s="37"/>
+      <c r="AZ17" s="37"/>
+      <c r="BA17" s="37"/>
+      <c r="BB17" s="37"/>
+      <c r="BC17" s="37"/>
+      <c r="BD17" s="37"/>
+      <c r="BE17" s="37"/>
+      <c r="BF17" s="37"/>
+      <c r="BG17" s="37"/>
+      <c r="BH17" s="37"/>
+      <c r="BI17" s="37"/>
+      <c r="BJ17" s="37"/>
+      <c r="BK17" s="37"/>
+      <c r="BL17" s="37"/>
+      <c r="BM17" s="37"/>
+      <c r="BN17" s="32"/>
     </row>
-    <row r="18" spans="1:66" s="51" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="46"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="50"/>
-      <c r="AA18" s="52"/>
-      <c r="AB18" s="52"/>
-      <c r="AC18" s="52"/>
-      <c r="AD18" s="52"/>
-      <c r="AE18" s="52"/>
-      <c r="AF18" s="52"/>
-      <c r="AG18" s="52"/>
-      <c r="AH18" s="52"/>
-      <c r="AI18" s="52"/>
-      <c r="AJ18" s="52"/>
-      <c r="AK18" s="52"/>
-      <c r="AL18" s="52"/>
-      <c r="AM18" s="52"/>
-      <c r="AN18" s="52"/>
-      <c r="AO18" s="52"/>
-      <c r="AP18" s="52"/>
-      <c r="AQ18" s="52"/>
-      <c r="AR18" s="52"/>
-      <c r="AS18" s="52"/>
-      <c r="AT18" s="52"/>
-      <c r="AU18" s="52"/>
-      <c r="AV18" s="52"/>
-      <c r="AW18" s="52"/>
-      <c r="AX18" s="52"/>
-      <c r="AY18" s="52"/>
-      <c r="AZ18" s="52"/>
-      <c r="BA18" s="52"/>
-      <c r="BB18" s="52"/>
-      <c r="BC18" s="52"/>
-      <c r="BD18" s="52"/>
-      <c r="BE18" s="52"/>
-      <c r="BF18" s="52"/>
-      <c r="BG18" s="52"/>
-      <c r="BH18" s="52"/>
-      <c r="BI18" s="52"/>
-      <c r="BJ18" s="52"/>
-      <c r="BK18" s="52"/>
-      <c r="BL18" s="52"/>
-      <c r="BM18" s="52"/>
-      <c r="BN18" s="52"/>
+    <row r="18" spans="1:66" s="43" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="38"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="42"/>
+      <c r="AA18" s="44"/>
+      <c r="AB18" s="44"/>
+      <c r="AC18" s="44"/>
+      <c r="AD18" s="44"/>
+      <c r="AE18" s="44"/>
+      <c r="AF18" s="44"/>
+      <c r="AG18" s="44"/>
+      <c r="AH18" s="44"/>
+      <c r="AI18" s="44"/>
+      <c r="AJ18" s="44"/>
+      <c r="AK18" s="44"/>
+      <c r="AL18" s="44"/>
+      <c r="AM18" s="44"/>
+      <c r="AN18" s="44"/>
+      <c r="AO18" s="44"/>
+      <c r="AP18" s="44"/>
+      <c r="AQ18" s="44"/>
+      <c r="AR18" s="44"/>
+      <c r="AS18" s="44"/>
+      <c r="AT18" s="44"/>
+      <c r="AU18" s="44"/>
+      <c r="AV18" s="44"/>
+      <c r="AW18" s="44"/>
+      <c r="AX18" s="44"/>
+      <c r="AY18" s="44"/>
+      <c r="AZ18" s="44"/>
+      <c r="BA18" s="44"/>
+      <c r="BB18" s="44"/>
+      <c r="BC18" s="44"/>
+      <c r="BD18" s="44"/>
+      <c r="BE18" s="44"/>
+      <c r="BF18" s="44"/>
+      <c r="BG18" s="44"/>
+      <c r="BH18" s="44"/>
+      <c r="BI18" s="44"/>
+      <c r="BJ18" s="44"/>
+      <c r="BK18" s="44"/>
+      <c r="BL18" s="44"/>
+      <c r="BM18" s="44"/>
+      <c r="BN18" s="44"/>
     </row>
-    <row r="19" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="13"/>
+    <row r="19" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="10"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -2503,13 +2503,13 @@
       <c r="BM19" s="3"/>
       <c r="BN19" s="3"/>
     </row>
-    <row r="20" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="13"/>
+    <row r="20" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -2571,13 +2571,13 @@
       <c r="BM20" s="3"/>
       <c r="BN20" s="3"/>
     </row>
-    <row r="21" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="13"/>
+    <row r="21" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="10"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -2639,13 +2639,13 @@
       <c r="BM21" s="3"/>
       <c r="BN21" s="3"/>
     </row>
-    <row r="22" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="13"/>
+    <row r="22" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -2707,13 +2707,13 @@
       <c r="BM22" s="3"/>
       <c r="BN22" s="3"/>
     </row>
-    <row r="23" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="13"/>
+    <row r="23" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="10"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -2775,13 +2775,13 @@
       <c r="BM23" s="3"/>
       <c r="BN23" s="3"/>
     </row>
-    <row r="24" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="13"/>
+    <row r="24" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="10"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -2843,13 +2843,13 @@
       <c r="BM24" s="3"/>
       <c r="BN24" s="3"/>
     </row>
-    <row r="25" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="13"/>
+    <row r="25" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -2911,13 +2911,13 @@
       <c r="BM25" s="3"/>
       <c r="BN25" s="3"/>
     </row>
-    <row r="26" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="13"/>
+    <row r="26" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="10"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -2979,13 +2979,13 @@
       <c r="BM26" s="3"/>
       <c r="BN26" s="3"/>
     </row>
-    <row r="27" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="13"/>
+    <row r="27" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -3047,13 +3047,13 @@
       <c r="BM27" s="3"/>
       <c r="BN27" s="3"/>
     </row>
-    <row r="28" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="13"/>
+    <row r="28" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="10"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -3115,13 +3115,13 @@
       <c r="BM28" s="3"/>
       <c r="BN28" s="3"/>
     </row>
-    <row r="29" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="13"/>
+    <row r="29" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="8"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="10"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -3183,150 +3183,150 @@
       <c r="BM29" s="3"/>
       <c r="BN29" s="3"/>
     </row>
-    <row r="30" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="128" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="130" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="132" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="133" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="134" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="135" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="136" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="137" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="138" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="139" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="140" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="141" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="145" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="146" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="147" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="148" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="149" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="150" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="151" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="152" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="154" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="155" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="160" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="161" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="162" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="163" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="164" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="165" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="166" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="167" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="168" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="169" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="170" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="171" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="172" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="173" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="31" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="32" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="34" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="35" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="36" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="37" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="38" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="39" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="40" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="41" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="42" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="43" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="44" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="45" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="46" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="47" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="48" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="49" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="50" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="51" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="52" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="53" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="54" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="55" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="56" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="57" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="58" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="59" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="60" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="61" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="62" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="63" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="64" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="65" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="66" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="67" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="68" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="69" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="70" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="71" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="72" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="73" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="74" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="75" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="76" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="77" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="78" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="79" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="80" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="81" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="82" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="83" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="84" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="85" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="86" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="87" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="88" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="89" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="90" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="91" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="92" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="93" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="94" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="95" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="96" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="97" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="98" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="99" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="100" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="101" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="102" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="103" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="104" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="105" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="106" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="107" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="108" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="109" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="110" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="111" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="112" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="113" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="114" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="115" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="116" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="117" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="118" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="119" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="120" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="121" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="122" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="123" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="124" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="125" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="126" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="127" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="128" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="129" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="130" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="131" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="132" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="133" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="134" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="135" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="136" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="137" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="138" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="139" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="140" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="141" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="142" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="143" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="144" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="145" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="146" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="147" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="148" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="149" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="150" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="151" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="152" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="153" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="154" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="155" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="156" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="157" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="158" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="159" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="160" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="161" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="162" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="163" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="164" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="165" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="166" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="167" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="168" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="169" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="170" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="171" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="172" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="173" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A1:XFD1"/>
@@ -3350,7 +3350,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="T2" xr:uid="{AF31CE32-1CA2-014D-AD02-59BB94C6851E}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="P2" xr:uid="{098B87B3-A0CB-244A-B2C1-AD633009B3A4}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="Q2 M2" xr:uid="{76B72423-F98A-C042-B383-44617B600B6E}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="J2 H5:H6 I7 H11 H14" xr:uid="{A199AD94-0335-F249-85C7-FA4FE53FA356}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="J2 H5:H6 I7 H11 H14 J15" xr:uid="{A199AD94-0335-F249-85C7-FA4FE53FA356}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="G2 L15 I8:K10 I12:K13 I5:I6 I14" xr:uid="{B12D7A5D-6678-2247-9E84-D505C287109C}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finished up milestone2 gantt chart
</commit_message>
<xml_diff>
--- a/Gantt Charts/Milestone2-GanttChart.xlsx
+++ b/Gantt Charts/Milestone2-GanttChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\OneDrive\Documents\Spring2020\CMPE 131\project\Calendar-Scheduling-app\Gantt Charts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shana/Desktop/CMPE 131/calApp/Calendar-Scheduling-App-master/Gantt Charts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{015F4838-0B26-E54F-9413-8DDD1BD8084A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{F697E4BB-999B-4743-B57D-2F47599D8B99}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A29982D-9C48-1848-9DBA-46D47FB78512}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="2160" windowWidth="28800" windowHeight="15435" xr2:uid="{AA7B69DF-3B17-C04C-9150-938323FE9379}"/>
+    <workbookView xWindow="100" yWindow="1020" windowWidth="28800" windowHeight="16920" xr2:uid="{AA7B69DF-3B17-C04C-9150-938323FE9379}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -309,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -534,32 +534,6 @@
       <top style="thin">
         <color theme="2" tint="-9.9978637043366805E-2"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0"/>
-      </left>
-      <right style="thick">
-        <color theme="0"/>
-      </right>
-      <top style="thick">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </top>
       <bottom style="thin">
         <color theme="0"/>
       </bottom>
@@ -576,6 +550,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -620,7 +631,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -768,41 +779,44 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="8" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="22" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="8" applyNumberFormat="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="24" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -1137,99 +1151,99 @@
   <dimension ref="A1:BN173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.25" style="4" customWidth="1"/>
-    <col min="2" max="3" width="10.875" style="4" customWidth="1"/>
-    <col min="4" max="6" width="10.875" style="4"/>
-    <col min="7" max="7" width="7.75" style="4" customWidth="1"/>
-    <col min="8" max="66" width="8.875" style="4" customWidth="1"/>
-    <col min="67" max="68" width="5.375" style="4" customWidth="1"/>
-    <col min="69" max="16384" width="10.875" style="4"/>
+    <col min="1" max="1" width="17.1640625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="4" customWidth="1"/>
+    <col min="4" max="6" width="10.83203125" style="4"/>
+    <col min="7" max="7" width="7.6640625" style="4" customWidth="1"/>
+    <col min="8" max="66" width="8.83203125" style="4" customWidth="1"/>
+    <col min="67" max="68" width="5.33203125" style="4" customWidth="1"/>
+    <col min="69" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="54" customFormat="1" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:66" s="53" customFormat="1" ht="64.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="55"/>
-      <c r="AI1" s="55"/>
-      <c r="AJ1" s="55"/>
-      <c r="AK1" s="55"/>
-      <c r="AL1" s="55"/>
-      <c r="AM1" s="55"/>
-      <c r="AN1" s="55"/>
-      <c r="AO1" s="55"/>
-      <c r="AP1" s="55"/>
-      <c r="AQ1" s="55"/>
-      <c r="AR1" s="55"/>
-      <c r="AS1" s="55"/>
-      <c r="AT1" s="55"/>
-      <c r="AU1" s="55"/>
-      <c r="AV1" s="55"/>
-      <c r="AW1" s="55"/>
-      <c r="AX1" s="55"/>
-      <c r="AY1" s="55"/>
-      <c r="AZ1" s="55"/>
-      <c r="BA1" s="55"/>
-      <c r="BB1" s="55"/>
-      <c r="BC1" s="55"/>
-      <c r="BD1" s="55"/>
-      <c r="BE1" s="55"/>
-      <c r="BF1" s="55"/>
-      <c r="BG1" s="55"/>
-      <c r="BH1" s="55"/>
-      <c r="BI1" s="55"/>
-      <c r="BJ1" s="55"/>
-      <c r="BK1" s="55"/>
-      <c r="BL1" s="55"/>
-      <c r="BM1" s="55"/>
-      <c r="BN1" s="55"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54"/>
+      <c r="AL1" s="54"/>
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="54"/>
+      <c r="AR1" s="54"/>
+      <c r="AS1" s="54"/>
+      <c r="AT1" s="54"/>
+      <c r="AU1" s="54"/>
+      <c r="AV1" s="54"/>
+      <c r="AW1" s="54"/>
+      <c r="AX1" s="54"/>
+      <c r="AY1" s="54"/>
+      <c r="AZ1" s="54"/>
+      <c r="BA1" s="54"/>
+      <c r="BB1" s="54"/>
+      <c r="BC1" s="54"/>
+      <c r="BD1" s="54"/>
+      <c r="BE1" s="54"/>
+      <c r="BF1" s="54"/>
+      <c r="BG1" s="54"/>
+      <c r="BH1" s="54"/>
+      <c r="BI1" s="54"/>
+      <c r="BJ1" s="54"/>
+      <c r="BK1" s="54"/>
+      <c r="BL1" s="54"/>
+      <c r="BM1" s="54"/>
+      <c r="BN1" s="54"/>
     </row>
-    <row r="2" spans="1:66" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="56" t="s">
+    <row r="2" spans="1:66" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="57"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56"/>
       <c r="G2" s="23"/>
       <c r="H2" s="14" t="s">
         <v>0</v>
@@ -1298,23 +1312,23 @@
       <c r="BM2" s="3"/>
       <c r="BN2" s="3"/>
     </row>
-    <row r="3" spans="1:66" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="60" t="s">
+    <row r="3" spans="1:66" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="F3" s="57" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="6"/>
@@ -1377,13 +1391,13 @@
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
     </row>
-    <row r="4" spans="1:66" ht="26.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="61"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
+    <row r="4" spans="1:66" ht="26" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="60"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
       <c r="G4" s="13">
         <v>43934</v>
       </c>
@@ -1459,7 +1473,7 @@
       <c r="BM4" s="12"/>
       <c r="BN4" s="12"/>
     </row>
-    <row r="5" spans="1:66" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:66" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
@@ -1469,12 +1483,16 @@
       <c r="C5" s="9">
         <v>2</v>
       </c>
-      <c r="D5" s="9">
-        <v>14</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="10"/>
-      <c r="H5" s="24"/>
+      <c r="D5" s="30">
+        <v>43935</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
+      <c r="H5" s="25"/>
       <c r="I5" s="2"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1534,7 +1552,7 @@
       <c r="BM5" s="3"/>
       <c r="BN5" s="3"/>
     </row>
-    <row r="6" spans="1:66" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:66" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="47"/>
       <c r="B6" s="30"/>
       <c r="C6" s="9"/>
@@ -1601,23 +1619,27 @@
       <c r="BM6" s="3"/>
       <c r="BN6" s="3"/>
     </row>
-    <row r="7" spans="1:66" ht="34.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:66" ht="38" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="9">
-        <v>15</v>
+      <c r="B7" s="30">
+        <v>43936</v>
       </c>
       <c r="C7" s="9">
         <v>1</v>
       </c>
-      <c r="D7" s="9">
-        <v>15</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="10"/>
+      <c r="D7" s="30">
+        <v>43936</v>
+      </c>
+      <c r="E7" s="9">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="24"/>
+      <c r="I7" s="25"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1676,23 +1698,29 @@
       <c r="BM7" s="3"/>
       <c r="BN7" s="3"/>
     </row>
-    <row r="8" spans="1:66" ht="34.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:66" ht="38" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="9">
-        <v>15</v>
+      <c r="B8" s="30">
+        <v>43936</v>
       </c>
       <c r="C8" s="9">
         <v>3</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="10"/>
+      <c r="D8" s="30">
+        <v>43938</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="K8" s="25"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1749,23 +1777,29 @@
       <c r="BM8" s="3"/>
       <c r="BN8" s="3"/>
     </row>
-    <row r="9" spans="1:66" ht="34.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:66" ht="38" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="9">
-        <v>15</v>
+      <c r="B9" s="30">
+        <v>43936</v>
       </c>
       <c r="C9" s="9">
         <v>3</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="10"/>
+      <c r="D9" s="30">
+        <v>43938</v>
+      </c>
+      <c r="E9" s="9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="10">
+        <v>1</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="K9" s="25"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1822,7 +1856,7 @@
       <c r="BM9" s="3"/>
       <c r="BN9" s="3"/>
     </row>
-    <row r="10" spans="1:66" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:66" ht="18" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -1889,25 +1923,29 @@
       <c r="BM10" s="3"/>
       <c r="BN10" s="3"/>
     </row>
-    <row r="11" spans="1:66" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:66" ht="55" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="9">
-        <v>14</v>
+      <c r="B11" s="30">
+        <v>43935</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
       </c>
-      <c r="D11" s="9">
-        <v>14</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="10"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
+      <c r="D11" s="30">
+        <v>43935</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="10">
+        <v>1</v>
+      </c>
+      <c r="H11" s="25"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -1964,23 +2002,29 @@
       <c r="BM11" s="3"/>
       <c r="BN11" s="3"/>
     </row>
-    <row r="12" spans="1:66" ht="67.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:66" ht="74" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="9">
-        <v>15</v>
+      <c r="B12" s="30">
+        <v>43936</v>
       </c>
       <c r="C12" s="9">
         <v>3</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="10"/>
+      <c r="D12" s="30">
+        <v>43938</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="K12" s="25"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -2037,17 +2081,17 @@
       <c r="BM12" s="3"/>
       <c r="BN12" s="3"/>
     </row>
-    <row r="13" spans="1:66" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:66" ht="20" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
-      <c r="F13" s="62"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="51"/>
+      <c r="F13" s="52"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -2104,26 +2148,30 @@
       <c r="BM13" s="3"/>
       <c r="BN13" s="3"/>
     </row>
-    <row r="14" spans="1:66" ht="34.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:66" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="9">
-        <v>14</v>
+      <c r="B14" s="30">
+        <v>43935</v>
       </c>
       <c r="C14" s="9">
         <v>2</v>
       </c>
-      <c r="D14" s="9">
-        <v>14</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="10"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="1"/>
+      <c r="D14" s="30">
+        <v>43935</v>
+      </c>
+      <c r="E14" s="9">
+        <v>6</v>
+      </c>
+      <c r="F14" s="10">
+        <v>1</v>
+      </c>
+      <c r="H14" s="63"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -2179,31 +2227,31 @@
       <c r="BM14" s="3"/>
       <c r="BN14" s="3"/>
     </row>
-    <row r="15" spans="1:66" ht="34.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:66" ht="38" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="30">
-        <v>43935</v>
+        <v>43937</v>
       </c>
       <c r="C15" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D15" s="30">
         <v>43937</v>
       </c>
       <c r="E15" s="9">
-        <v>2</v>
-      </c>
-      <c r="F15" s="62">
+        <v>3</v>
+      </c>
+      <c r="F15" s="10">
         <v>1</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -2258,7 +2306,7 @@
       <c r="BM15" s="3"/>
       <c r="BN15" s="3"/>
     </row>
-    <row r="16" spans="1:66" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:66" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -2326,7 +2374,7 @@
       <c r="BM16" s="3"/>
       <c r="BN16" s="3"/>
     </row>
-    <row r="17" spans="1:66" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:66" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="34"/>
       <c r="B17" s="31"/>
       <c r="C17" s="31"/>
@@ -2394,7 +2442,7 @@
       <c r="BM17" s="37"/>
       <c r="BN17" s="32"/>
     </row>
-    <row r="18" spans="1:66" s="43" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:66" s="43" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="38"/>
       <c r="B18" s="39"/>
       <c r="C18" s="40"/>
@@ -2442,7 +2490,7 @@
       <c r="BM18" s="44"/>
       <c r="BN18" s="44"/>
     </row>
-    <row r="19" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -2510,7 +2558,7 @@
       <c r="BM19" s="3"/>
       <c r="BN19" s="3"/>
     </row>
-    <row r="20" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -2578,7 +2626,7 @@
       <c r="BM20" s="3"/>
       <c r="BN20" s="3"/>
     </row>
-    <row r="21" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -2646,7 +2694,7 @@
       <c r="BM21" s="3"/>
       <c r="BN21" s="3"/>
     </row>
-    <row r="22" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -2714,7 +2762,7 @@
       <c r="BM22" s="3"/>
       <c r="BN22" s="3"/>
     </row>
-    <row r="23" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -2782,7 +2830,7 @@
       <c r="BM23" s="3"/>
       <c r="BN23" s="3"/>
     </row>
-    <row r="24" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -2850,7 +2898,7 @@
       <c r="BM24" s="3"/>
       <c r="BN24" s="3"/>
     </row>
-    <row r="25" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -2918,7 +2966,7 @@
       <c r="BM25" s="3"/>
       <c r="BN25" s="3"/>
     </row>
-    <row r="26" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -2986,7 +3034,7 @@
       <c r="BM26" s="3"/>
       <c r="BN26" s="3"/>
     </row>
-    <row r="27" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -3054,7 +3102,7 @@
       <c r="BM27" s="3"/>
       <c r="BN27" s="3"/>
     </row>
-    <row r="28" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -3122,7 +3170,7 @@
       <c r="BM28" s="3"/>
       <c r="BN28" s="3"/>
     </row>
-    <row r="29" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -3190,150 +3238,150 @@
       <c r="BM29" s="3"/>
       <c r="BN29" s="3"/>
     </row>
-    <row r="30" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A1:XFD1"/>
@@ -3354,11 +3402,11 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="C3:C4" xr:uid="{9EF1E97C-CF64-7948-A8CD-EA30BA312303}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="B3:B4" xr:uid="{8971EE31-53FE-6F44-A4E7-A0061F08C39F}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="A3:A4" xr:uid="{DE19D017-F753-9340-9B91-166526B028E1}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="T2" xr:uid="{AF31CE32-1CA2-014D-AD02-59BB94C6851E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="T2 J14:L14" xr:uid="{AF31CE32-1CA2-014D-AD02-59BB94C6851E}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="P2" xr:uid="{098B87B3-A0CB-244A-B2C1-AD633009B3A4}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="Q2 M2 M15" xr:uid="{76B72423-F98A-C042-B383-44617B600B6E}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="J2 H5:H6 I7 H11 H14 J15" xr:uid="{A199AD94-0335-F249-85C7-FA4FE53FA356}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="G2 I14 I8:K10 I12:K13 I5:I6 K15:L15" xr:uid="{B12D7A5D-6678-2247-9E84-D505C287109C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="Q2 M2 H14:I14 H11 K12 K8:K9 I7 H5 J15:L15" xr:uid="{76B72423-F98A-C042-B383-44617B600B6E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="J2 H6" xr:uid="{A199AD94-0335-F249-85C7-FA4FE53FA356}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="G2 I12:J12 I8:J10 K10 I5:I6" xr:uid="{B12D7A5D-6678-2247-9E84-D505C287109C}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' into temp"
This reverts commit dce2bfa62105b46145430159e1c0aa3361fbfb72, reversing
changes made to 544cbd799801a80a11c439c1a6ad891d9e4341b1.
</commit_message>
<xml_diff>
--- a/Gantt Charts/Milestone2-GanttChart.xlsx
+++ b/Gantt Charts/Milestone2-GanttChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/de594e4e93e79e7e/Documents/Spring2020/CMPE 131/project/Calendar-Scheduling-app/Gantt Charts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shana/Desktop/CMPE 131/calApp/Calendar-Scheduling-App-master/Gantt Charts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{015F4838-0B26-E54F-9413-8DDD1BD8084A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F72D0CBE-E9BB-4966-B2EA-4E931021CABE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A29982D-9C48-1848-9DBA-46D47FB78512}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2123" yWindow="2242" windowWidth="16874" windowHeight="10523" xr2:uid="{AA7B69DF-3B17-C04C-9150-938323FE9379}"/>
+    <workbookView xWindow="100" yWindow="1020" windowWidth="28800" windowHeight="16920" xr2:uid="{AA7B69DF-3B17-C04C-9150-938323FE9379}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -311,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -536,32 +534,6 @@
       <top style="thin">
         <color theme="2" tint="-9.9978637043366805E-2"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0"/>
-      </left>
-      <right style="thick">
-        <color theme="0"/>
-      </right>
-      <top style="thick">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </top>
       <bottom style="thin">
         <color theme="0"/>
       </bottom>
@@ -578,6 +550,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -622,7 +631,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -770,38 +779,44 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="8" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="22" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="24" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -1135,100 +1150,100 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382B5C2B-D08E-CD4E-BF62-F343AB5B8050}">
   <dimension ref="A1:BN173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1875" style="4" customWidth="1"/>
-    <col min="2" max="3" width="10.8125" style="4" customWidth="1"/>
-    <col min="4" max="6" width="10.8125" style="4"/>
-    <col min="7" max="7" width="7.6875" style="4" customWidth="1"/>
-    <col min="8" max="66" width="8.8125" style="4" customWidth="1"/>
-    <col min="67" max="68" width="5.3125" style="4" customWidth="1"/>
-    <col min="69" max="16384" width="10.8125" style="4"/>
+    <col min="1" max="1" width="17.1640625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="4" customWidth="1"/>
+    <col min="4" max="6" width="10.83203125" style="4"/>
+    <col min="7" max="7" width="7.6640625" style="4" customWidth="1"/>
+    <col min="8" max="66" width="8.83203125" style="4" customWidth="1"/>
+    <col min="67" max="68" width="5.33203125" style="4" customWidth="1"/>
+    <col min="69" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="54" customFormat="1" ht="64.05" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:66" s="53" customFormat="1" ht="64.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="55"/>
-      <c r="AI1" s="55"/>
-      <c r="AJ1" s="55"/>
-      <c r="AK1" s="55"/>
-      <c r="AL1" s="55"/>
-      <c r="AM1" s="55"/>
-      <c r="AN1" s="55"/>
-      <c r="AO1" s="55"/>
-      <c r="AP1" s="55"/>
-      <c r="AQ1" s="55"/>
-      <c r="AR1" s="55"/>
-      <c r="AS1" s="55"/>
-      <c r="AT1" s="55"/>
-      <c r="AU1" s="55"/>
-      <c r="AV1" s="55"/>
-      <c r="AW1" s="55"/>
-      <c r="AX1" s="55"/>
-      <c r="AY1" s="55"/>
-      <c r="AZ1" s="55"/>
-      <c r="BA1" s="55"/>
-      <c r="BB1" s="55"/>
-      <c r="BC1" s="55"/>
-      <c r="BD1" s="55"/>
-      <c r="BE1" s="55"/>
-      <c r="BF1" s="55"/>
-      <c r="BG1" s="55"/>
-      <c r="BH1" s="55"/>
-      <c r="BI1" s="55"/>
-      <c r="BJ1" s="55"/>
-      <c r="BK1" s="55"/>
-      <c r="BL1" s="55"/>
-      <c r="BM1" s="55"/>
-      <c r="BN1" s="55"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54"/>
+      <c r="AL1" s="54"/>
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="54"/>
+      <c r="AR1" s="54"/>
+      <c r="AS1" s="54"/>
+      <c r="AT1" s="54"/>
+      <c r="AU1" s="54"/>
+      <c r="AV1" s="54"/>
+      <c r="AW1" s="54"/>
+      <c r="AX1" s="54"/>
+      <c r="AY1" s="54"/>
+      <c r="AZ1" s="54"/>
+      <c r="BA1" s="54"/>
+      <c r="BB1" s="54"/>
+      <c r="BC1" s="54"/>
+      <c r="BD1" s="54"/>
+      <c r="BE1" s="54"/>
+      <c r="BF1" s="54"/>
+      <c r="BG1" s="54"/>
+      <c r="BH1" s="54"/>
+      <c r="BI1" s="54"/>
+      <c r="BJ1" s="54"/>
+      <c r="BK1" s="54"/>
+      <c r="BL1" s="54"/>
+      <c r="BM1" s="54"/>
+      <c r="BN1" s="54"/>
     </row>
-    <row r="2" spans="1:66" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="56" t="s">
+    <row r="2" spans="1:66" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="57"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56"/>
       <c r="G2" s="23"/>
       <c r="H2" s="14" t="s">
         <v>0</v>
@@ -1297,23 +1312,23 @@
       <c r="BM2" s="3"/>
       <c r="BN2" s="3"/>
     </row>
-    <row r="3" spans="1:66" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="60" t="s">
+    <row r="3" spans="1:66" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="F3" s="57" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="6"/>
@@ -1376,13 +1391,13 @@
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
     </row>
-    <row r="4" spans="1:66" ht="26" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="61"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
+    <row r="4" spans="1:66" ht="26" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="60"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
       <c r="G4" s="13">
         <v>43934</v>
       </c>
@@ -1458,7 +1473,7 @@
       <c r="BM4" s="12"/>
       <c r="BN4" s="12"/>
     </row>
-    <row r="5" spans="1:66" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:66" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
@@ -1468,12 +1483,16 @@
       <c r="C5" s="9">
         <v>2</v>
       </c>
-      <c r="D5" s="9">
-        <v>14</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="10"/>
-      <c r="H5" s="24"/>
+      <c r="D5" s="30">
+        <v>43935</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
+      <c r="H5" s="25"/>
       <c r="I5" s="2"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1533,7 +1552,7 @@
       <c r="BM5" s="3"/>
       <c r="BN5" s="3"/>
     </row>
-    <row r="6" spans="1:66" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:66" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="47"/>
       <c r="B6" s="30"/>
       <c r="C6" s="9"/>
@@ -1600,23 +1619,27 @@
       <c r="BM6" s="3"/>
       <c r="BN6" s="3"/>
     </row>
-    <row r="7" spans="1:66" ht="33.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:66" ht="38" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="9">
-        <v>15</v>
+      <c r="B7" s="30">
+        <v>43936</v>
       </c>
       <c r="C7" s="9">
         <v>1</v>
       </c>
-      <c r="D7" s="9">
-        <v>15</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="10"/>
+      <c r="D7" s="30">
+        <v>43936</v>
+      </c>
+      <c r="E7" s="9">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="24"/>
+      <c r="I7" s="25"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1675,23 +1698,29 @@
       <c r="BM7" s="3"/>
       <c r="BN7" s="3"/>
     </row>
-    <row r="8" spans="1:66" ht="33.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:66" ht="38" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="9">
-        <v>15</v>
+      <c r="B8" s="30">
+        <v>43936</v>
       </c>
       <c r="C8" s="9">
         <v>3</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="10"/>
+      <c r="D8" s="30">
+        <v>43938</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="K8" s="25"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1748,23 +1777,29 @@
       <c r="BM8" s="3"/>
       <c r="BN8" s="3"/>
     </row>
-    <row r="9" spans="1:66" ht="33.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:66" ht="38" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="9">
-        <v>15</v>
+      <c r="B9" s="30">
+        <v>43936</v>
       </c>
       <c r="C9" s="9">
         <v>3</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="10"/>
+      <c r="D9" s="30">
+        <v>43938</v>
+      </c>
+      <c r="E9" s="9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="10">
+        <v>1</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="K9" s="25"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1821,7 +1856,7 @@
       <c r="BM9" s="3"/>
       <c r="BN9" s="3"/>
     </row>
-    <row r="10" spans="1:66" ht="16.899999999999999" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:66" ht="18" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -1888,25 +1923,29 @@
       <c r="BM10" s="3"/>
       <c r="BN10" s="3"/>
     </row>
-    <row r="11" spans="1:66" ht="49.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:66" ht="55" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="9">
-        <v>14</v>
+      <c r="B11" s="30">
+        <v>43935</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
       </c>
-      <c r="D11" s="9">
-        <v>14</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="10"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
+      <c r="D11" s="30">
+        <v>43935</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="10">
+        <v>1</v>
+      </c>
+      <c r="H11" s="25"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -1963,23 +2002,29 @@
       <c r="BM11" s="3"/>
       <c r="BN11" s="3"/>
     </row>
-    <row r="12" spans="1:66" ht="66.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:66" ht="74" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="9">
-        <v>15</v>
+      <c r="B12" s="30">
+        <v>43936</v>
       </c>
       <c r="C12" s="9">
         <v>3</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="10"/>
+      <c r="D12" s="30">
+        <v>43938</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="K12" s="25"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -2036,17 +2081,17 @@
       <c r="BM12" s="3"/>
       <c r="BN12" s="3"/>
     </row>
-    <row r="13" spans="1:66" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:66" ht="20" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
-      <c r="F13" s="10"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="51"/>
+      <c r="F13" s="52"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -2103,26 +2148,30 @@
       <c r="BM13" s="3"/>
       <c r="BN13" s="3"/>
     </row>
-    <row r="14" spans="1:66" ht="33.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:66" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="9">
-        <v>14</v>
+      <c r="B14" s="30">
+        <v>43935</v>
       </c>
       <c r="C14" s="9">
         <v>2</v>
       </c>
-      <c r="D14" s="9">
-        <v>14</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="10"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="1"/>
+      <c r="D14" s="30">
+        <v>43935</v>
+      </c>
+      <c r="E14" s="9">
+        <v>6</v>
+      </c>
+      <c r="F14" s="10">
+        <v>1</v>
+      </c>
+      <c r="H14" s="63"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -2178,24 +2227,30 @@
       <c r="BM14" s="3"/>
       <c r="BN14" s="3"/>
     </row>
-    <row r="15" spans="1:66" ht="33.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:66" ht="38" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="9">
-        <v>18</v>
+      <c r="B15" s="30">
+        <v>43937</v>
       </c>
       <c r="C15" s="9">
+        <v>3</v>
+      </c>
+      <c r="D15" s="30">
+        <v>43937</v>
+      </c>
+      <c r="E15" s="9">
+        <v>3</v>
+      </c>
+      <c r="F15" s="10">
         <v>1</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="10"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="2"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -2251,7 +2306,7 @@
       <c r="BM15" s="3"/>
       <c r="BN15" s="3"/>
     </row>
-    <row r="16" spans="1:66" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:66" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -2319,7 +2374,7 @@
       <c r="BM16" s="3"/>
       <c r="BN16" s="3"/>
     </row>
-    <row r="17" spans="1:66" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:66" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="34"/>
       <c r="B17" s="31"/>
       <c r="C17" s="31"/>
@@ -2387,7 +2442,7 @@
       <c r="BM17" s="37"/>
       <c r="BN17" s="32"/>
     </row>
-    <row r="18" spans="1:66" s="43" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:66" s="43" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="38"/>
       <c r="B18" s="39"/>
       <c r="C18" s="40"/>
@@ -2435,7 +2490,7 @@
       <c r="BM18" s="44"/>
       <c r="BN18" s="44"/>
     </row>
-    <row r="19" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -2503,7 +2558,7 @@
       <c r="BM19" s="3"/>
       <c r="BN19" s="3"/>
     </row>
-    <row r="20" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -2571,7 +2626,7 @@
       <c r="BM20" s="3"/>
       <c r="BN20" s="3"/>
     </row>
-    <row r="21" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -2639,7 +2694,7 @@
       <c r="BM21" s="3"/>
       <c r="BN21" s="3"/>
     </row>
-    <row r="22" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -2707,7 +2762,7 @@
       <c r="BM22" s="3"/>
       <c r="BN22" s="3"/>
     </row>
-    <row r="23" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -2775,7 +2830,7 @@
       <c r="BM23" s="3"/>
       <c r="BN23" s="3"/>
     </row>
-    <row r="24" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -2843,7 +2898,7 @@
       <c r="BM24" s="3"/>
       <c r="BN24" s="3"/>
     </row>
-    <row r="25" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -2911,7 +2966,7 @@
       <c r="BM25" s="3"/>
       <c r="BN25" s="3"/>
     </row>
-    <row r="26" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -2979,7 +3034,7 @@
       <c r="BM26" s="3"/>
       <c r="BN26" s="3"/>
     </row>
-    <row r="27" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -3047,7 +3102,7 @@
       <c r="BM27" s="3"/>
       <c r="BN27" s="3"/>
     </row>
-    <row r="28" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -3115,7 +3170,7 @@
       <c r="BM28" s="3"/>
       <c r="BN28" s="3"/>
     </row>
-    <row r="29" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -3183,150 +3238,150 @@
       <c r="BM29" s="3"/>
       <c r="BN29" s="3"/>
     </row>
-    <row r="30" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="31" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="32" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="34" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="35" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="36" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="37" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="38" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="39" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="40" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="41" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="42" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="43" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="44" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="45" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="46" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="47" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="48" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="49" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="50" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="51" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="52" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="53" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="54" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="55" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="56" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="57" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="58" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="59" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="60" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="61" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="62" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="63" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="64" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="65" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="66" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="67" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="68" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="69" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="70" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="71" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="72" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="73" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="74" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="75" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="76" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="77" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="78" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="79" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="80" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="81" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="82" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="83" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="84" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="85" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="86" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="87" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="88" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="89" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="90" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="91" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="92" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="93" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="94" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="95" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="96" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="97" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="98" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="99" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="100" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="101" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="102" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="103" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="104" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="105" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="106" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="107" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="108" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="109" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="110" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="111" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="112" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="113" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="114" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="115" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="116" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="117" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="118" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="119" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="120" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="121" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="122" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="123" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="124" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="125" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="126" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="127" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="128" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="129" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="130" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="131" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="132" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="133" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="134" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="135" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="136" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="137" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="138" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="139" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="140" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="141" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="142" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="143" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="144" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="145" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="146" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="147" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="148" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="149" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="150" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="151" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="152" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="153" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="154" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="155" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="156" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="157" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="158" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="159" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="160" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="161" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="162" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="163" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="164" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="165" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="166" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="167" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="168" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="169" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="170" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="171" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="172" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="173" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="30" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A1:XFD1"/>
@@ -3347,11 +3402,11 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="C3:C4" xr:uid="{9EF1E97C-CF64-7948-A8CD-EA30BA312303}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="B3:B4" xr:uid="{8971EE31-53FE-6F44-A4E7-A0061F08C39F}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="A3:A4" xr:uid="{DE19D017-F753-9340-9B91-166526B028E1}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="T2" xr:uid="{AF31CE32-1CA2-014D-AD02-59BB94C6851E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="T2 J14:L14" xr:uid="{AF31CE32-1CA2-014D-AD02-59BB94C6851E}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="P2" xr:uid="{098B87B3-A0CB-244A-B2C1-AD633009B3A4}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="Q2 M2" xr:uid="{76B72423-F98A-C042-B383-44617B600B6E}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="J2 H5:H6 I7 H11 H14 J15" xr:uid="{A199AD94-0335-F249-85C7-FA4FE53FA356}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="G2 L15 I8:K10 I12:K13 I5:I6 I14" xr:uid="{B12D7A5D-6678-2247-9E84-D505C287109C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="Q2 M2 H14:I14 H11 K12 K8:K9 I7 H5 J15:L15" xr:uid="{76B72423-F98A-C042-B383-44617B600B6E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="J2 H6" xr:uid="{A199AD94-0335-F249-85C7-FA4FE53FA356}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="G2 I12:J12 I8:J10 K10 I5:I6" xr:uid="{B12D7A5D-6678-2247-9E84-D505C287109C}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>